<commit_message>
Update Fashion Models & Overview
</commit_message>
<xml_diff>
--- a/$AEO.xlsx
+++ b/$AEO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC78A3E8-BCD9-4020-8B82-A928574215A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42C7B63-49CA-49DC-9AAA-C0FC50D8CA0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="30765" windowHeight="18900" xr2:uid="{2D5D8E9F-9DBA-4771-9CE7-44578AC3E7E6}"/>
   </bookViews>
@@ -714,16 +714,10 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -735,22 +729,28 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1242,7 +1242,7 @@
   <dimension ref="A2:R40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1262,31 +1262,31 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="49"/>
-      <c r="H5" s="47" t="s">
+      <c r="C5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="H5" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="49"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="47"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="4">
-        <v>10.24</v>
+        <v>12.92</v>
       </c>
       <c r="D6" s="9"/>
       <c r="H6" s="35"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="C8" s="33">
         <f>C6*C7</f>
-        <v>1725.0304000000001</v>
+        <v>2176.5032000000001</v>
       </c>
       <c r="D8" s="9"/>
       <c r="H8" s="35"/>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="C12" s="34">
         <f>C8-C11</f>
-        <v>1902.0304000000001</v>
+        <v>2353.5032000000001</v>
       </c>
       <c r="D12" s="10"/>
       <c r="H12" s="35"/>
@@ -1465,11 +1465,11 @@
       <c r="R14" s="12"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="47"/>
       <c r="H15" s="35"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
@@ -1489,10 +1489,10 @@
       <c r="B16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="44"/>
+      <c r="D16" s="49"/>
       <c r="H16" s="35"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
@@ -1512,10 +1512,10 @@
       <c r="B17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="44"/>
+      <c r="D17" s="49"/>
       <c r="H17" s="35"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
@@ -1530,8 +1530,8 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B18" s="7"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="44"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="49"/>
       <c r="H18" s="35"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
@@ -1546,8 +1546,8 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B19" s="8"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="53"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="44"/>
       <c r="H19" s="37"/>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
@@ -1561,147 +1561,155 @@
       <c r="R19" s="14"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="47"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B23" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="43" t="s">
+      <c r="C23" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="44"/>
+      <c r="D23" s="49"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B24" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="43">
+      <c r="C24" s="48">
         <v>1977</v>
       </c>
-      <c r="D24" s="44"/>
+      <c r="D24" s="49"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B25" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="50">
+      <c r="C25" s="54">
         <v>1141</v>
       </c>
-      <c r="D25" s="51"/>
+      <c r="D25" s="55"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B26" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="43">
+      <c r="C26" s="48">
         <f>'Financial Model'!O42</f>
         <v>682.1</v>
       </c>
-      <c r="D26" s="44"/>
+      <c r="D26" s="49"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B27" s="15"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="44"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="49"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B28" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="43" t="s">
+      <c r="C28" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="44"/>
+      <c r="D28" s="49"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B29" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="45" t="s">
+      <c r="C29" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="46"/>
+      <c r="D29" s="53"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B32" s="47" t="s">
+      <c r="B32" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="48"/>
-      <c r="D32" s="49"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="47"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C33" s="54">
+      <c r="C33" s="50">
         <f>C12/'Financial Model'!O16</f>
-        <v>59.925343415248761</v>
-      </c>
-      <c r="D33" s="55"/>
+        <v>74.149439193446582</v>
+      </c>
+      <c r="D33" s="51"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="54">
+      <c r="C34" s="50">
         <f>C6/'Financial Model'!Z17</f>
-        <v>4.0901579978361697</v>
-      </c>
-      <c r="D34" s="55"/>
+        <v>5.160629036332355</v>
+      </c>
+      <c r="D34" s="51"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="44"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="49"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="54">
+      <c r="C36" s="50">
         <f>C6/'Financial Model'!O69</f>
-        <v>1.2473050731522497</v>
-      </c>
-      <c r="D36" s="55"/>
+        <v>1.573748197766315</v>
+      </c>
+      <c r="D36" s="51"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="15"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="44"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="49"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="43"/>
-      <c r="D38" s="44"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="49"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="54">
+      <c r="C39" s="50">
         <f>C12/'Financial Model'!K16</f>
-        <v>19.924268041021126</v>
-      </c>
-      <c r="D39" s="55"/>
+        <v>24.653564208122514</v>
+      </c>
+      <c r="D39" s="51"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C40" s="52"/>
-      <c r="D40" s="53"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="H5:R5"/>
     <mergeCell ref="C35:D35"/>
@@ -1718,14 +1726,6 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{7B647FD1-964F-4B61-9B8A-709E47541E36}"/>

</xml_diff>

<commit_message>
More fashion retailer ROCE metrics
</commit_message>
<xml_diff>
--- a/$AEO.xlsx
+++ b/$AEO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCFBF2D-D256-4BDB-9F34-0589B3301328}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FBA370-5912-0745-8D9C-B1C44F8D7001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="30765" windowHeight="18900" activeTab="1" xr2:uid="{2D5D8E9F-9DBA-4771-9CE7-44578AC3E7E6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30760" windowHeight="18900" xr2:uid="{2D5D8E9F-9DBA-4771-9CE7-44578AC3E7E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="140">
   <si>
     <t>$AEO</t>
   </si>
@@ -654,7 +664,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -739,16 +749,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -760,16 +769,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -778,15 +781,26 @@
     <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -885,7 +899,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>92</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -935,7 +949,7 @@
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>92</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1277,47 +1291,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{188BF81D-3479-40A6-AF7B-7D17D51D3E4F}">
   <dimension ref="A2:R40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36:D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35:D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B5" s="48" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="B5" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="50"/>
-      <c r="H5" s="48" t="s">
+      <c r="C5" s="50"/>
+      <c r="D5" s="51"/>
+      <c r="H5" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="49"/>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="49"/>
-      <c r="R5" s="50"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="51"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1337,7 +1351,7 @@
       <c r="Q6" s="11"/>
       <c r="R6" s="12"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
@@ -1364,7 +1378,7 @@
       <c r="Q7" s="11"/>
       <c r="R7" s="12"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
@@ -1387,7 +1401,7 @@
       <c r="Q8" s="11"/>
       <c r="R8" s="12"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
@@ -1410,7 +1424,7 @@
       <c r="Q9" s="11"/>
       <c r="R9" s="12"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
@@ -1433,7 +1447,7 @@
       <c r="Q10" s="11"/>
       <c r="R10" s="12"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
@@ -1456,7 +1470,7 @@
       <c r="Q11" s="11"/>
       <c r="R11" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
@@ -1477,7 +1491,7 @@
       <c r="Q12" s="11"/>
       <c r="R12" s="12"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="H13" s="35"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
@@ -1490,7 +1504,7 @@
       <c r="Q13" s="11"/>
       <c r="R13" s="12"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="H14" s="35"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
@@ -1503,12 +1517,12 @@
       <c r="Q14" s="11"/>
       <c r="R14" s="12"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="48" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="B15" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
       <c r="H15" s="35"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
@@ -1521,17 +1535,17 @@
       <c r="Q15" s="11"/>
       <c r="R15" s="12"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="21" t="s">
         <v>83</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="45"/>
+      <c r="D16" s="53"/>
       <c r="H16" s="35"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
@@ -1544,17 +1558,17 @@
       <c r="Q16" s="11"/>
       <c r="R16" s="12"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="21" t="s">
         <v>84</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="45"/>
+      <c r="D17" s="53"/>
       <c r="H17" s="35"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
@@ -1567,10 +1581,10 @@
       <c r="Q17" s="11"/>
       <c r="R17" s="12"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B18" s="7"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="45"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="53"/>
       <c r="H18" s="35"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
@@ -1583,10 +1597,10 @@
       <c r="Q18" s="11"/>
       <c r="R18" s="12"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B19" s="8"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="54"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
       <c r="H19" s="37"/>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
@@ -1599,42 +1613,42 @@
       <c r="Q19" s="13"/>
       <c r="R19" s="14"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B22" s="48" t="s">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="B22" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="49"/>
-      <c r="D22" s="50"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C22" s="50"/>
+      <c r="D22" s="51"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B23" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="45"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D23" s="53"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B24" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="44">
+      <c r="C24" s="52">
         <v>1977</v>
       </c>
-      <c r="D24" s="45"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D24" s="53"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B25" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="51">
+      <c r="C25" s="58">
         <f>'Financial Model'!P38</f>
         <v>1160</v>
       </c>
-      <c r="D25" s="52"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D25" s="59"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B26" s="15" t="s">
         <v>17</v>
       </c>
@@ -1644,109 +1658,119 @@
       </c>
       <c r="D26" s="61"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B27" s="15"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="45"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C27" s="52"/>
+      <c r="D27" s="53"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B28" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="57">
+      <c r="D28" s="44">
         <v>44811</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B29" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="46" t="s">
+      <c r="C29" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="47"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B32" s="48" t="s">
+      <c r="D29" s="57"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="B32" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="49"/>
-      <c r="D32" s="50"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C32" s="50"/>
+      <c r="D32" s="51"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C33" s="55">
+      <c r="C33" s="54">
         <f>C12/SUM('Financial Model'!L17:P17)</f>
         <v>8.3153867603378018</v>
       </c>
-      <c r="D33" s="56"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="55"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B34" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="55">
+      <c r="C34" s="54">
         <f>C6/SUM('Financial Model'!M18:P18)</f>
         <v>11.122029267148672</v>
       </c>
-      <c r="D34" s="56"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D34" s="55"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="45"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C35" s="63">
+        <f>'Financial Model'!P88</f>
+        <v>0.25169437761622476</v>
+      </c>
+      <c r="D35" s="53"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B36" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="55">
+      <c r="C36" s="54">
         <f>C6/'Financial Model'!P70</f>
         <v>1.6956827731781026</v>
       </c>
-      <c r="D36" s="56"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D36" s="55"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B37" s="15"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="45"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C37" s="52"/>
+      <c r="D37" s="53"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B38" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="55">
+      <c r="C38" s="54">
         <f>'Financial Model'!Z86</f>
         <v>8.8873061964701936</v>
       </c>
-      <c r="D38" s="56"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D38" s="55"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B39" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="55">
+      <c r="C39" s="54">
         <f>'Financial Model'!Z87</f>
         <v>8.663850071253929</v>
       </c>
-      <c r="D39" s="56"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D39" s="55"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B40" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C40" s="53"/>
-      <c r="D40" s="54"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="H5:R5"/>
     <mergeCell ref="C35:D35"/>
@@ -1763,13 +1787,6 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{7B647FD1-964F-4B61-9B8A-709E47541E36}"/>
@@ -1782,23 +1799,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCAE567-3C76-461E-8871-8262189BBFA2}">
-  <dimension ref="A1:AN89"/>
+  <dimension ref="A1:AN90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C47" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="E72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C89" sqref="C89"/>
+      <selection pane="bottomRight" activeCell="N99" sqref="N99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:40" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:40" s="17" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C1" s="17" t="s">
         <v>21</v>
       </c>
@@ -1911,7 +1928,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="2:40" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:40" s="22" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B2" s="23"/>
       <c r="C2" s="24">
         <v>43589</v>
@@ -1962,7 +1979,7 @@
         <v>44590</v>
       </c>
     </row>
-    <row r="3" spans="2:40" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:40" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B3" s="38" t="s">
         <v>58</v>
       </c>
@@ -2013,7 +2030,7 @@
         <v>3557.84</v>
       </c>
     </row>
-    <row r="4" spans="2:40" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:40" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B4" s="38" t="s">
         <v>59</v>
       </c>
@@ -2064,7 +2081,7 @@
         <v>1376.749</v>
       </c>
     </row>
-    <row r="5" spans="2:40" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:40" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B5" s="38" t="s">
         <v>60</v>
       </c>
@@ -2115,7 +2132,7 @@
         <v>76.195999999999998</v>
       </c>
     </row>
-    <row r="6" spans="2:40" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:40" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B6" s="2" t="s">
         <v>61</v>
       </c>
@@ -2173,7 +2190,7 @@
         <v>5010.7849999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
         <v>62</v>
       </c>
@@ -2222,7 +2239,7 @@
         <v>3018.9949999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:40" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:40" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
         <v>63</v>
       </c>
@@ -2283,7 +2300,7 @@
         <v>1991.79</v>
       </c>
     </row>
-    <row r="9" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
         <v>64</v>
       </c>
@@ -2332,7 +2349,7 @@
         <v>1222.001</v>
       </c>
     </row>
-    <row r="10" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
         <v>65</v>
       </c>
@@ -2388,7 +2405,7 @@
         <v>178.72500000000002</v>
       </c>
     </row>
-    <row r="11" spans="2:40" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:40" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
         <v>66</v>
       </c>
@@ -2449,7 +2466,7 @@
         <v>591.06399999999996</v>
       </c>
     </row>
-    <row r="12" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
         <v>135</v>
       </c>
@@ -2502,7 +2519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
         <v>67</v>
       </c>
@@ -2552,7 +2569,7 @@
         <v>34.634</v>
       </c>
     </row>
-    <row r="14" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
         <v>68</v>
       </c>
@@ -2601,7 +2618,7 @@
         <v>-2.4879999999999995</v>
       </c>
     </row>
-    <row r="15" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
         <v>69</v>
       </c>
@@ -2662,7 +2679,7 @@
         <v>558.91799999999989</v>
       </c>
     </row>
-    <row r="16" spans="2:40" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:40" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
         <v>70</v>
       </c>
@@ -2712,7 +2729,7 @@
         <v>139.292</v>
       </c>
     </row>
-    <row r="17" spans="2:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:26" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B17" s="2" t="s">
         <v>71</v>
       </c>
@@ -2773,7 +2790,7 @@
         <v>419.62599999999986</v>
       </c>
     </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
         <v>72</v>
       </c>
@@ -2834,7 +2851,7 @@
         <v>2.5035707680283505</v>
       </c>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
@@ -2883,7 +2900,7 @@
         <v>167.61099999999999</v>
       </c>
     </row>
-    <row r="21" spans="2:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:26" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
         <v>73</v>
       </c>
@@ -2920,7 +2937,7 @@
         <v>0.33299379683036578</v>
       </c>
     </row>
-    <row r="22" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
         <v>74</v>
       </c>
@@ -2929,43 +2946,43 @@
         <v>0.17442259305644869</v>
       </c>
       <c r="H22" s="29">
-        <f>H6/G6-1</f>
+        <f t="shared" ref="H22:O22" si="12">H6/G6-1</f>
         <v>0.60145515976305619</v>
       </c>
       <c r="I22" s="29">
-        <f>I6/H6-1</f>
+        <f t="shared" si="12"/>
         <v>0.16763477493180612</v>
       </c>
       <c r="J22" s="29">
-        <f>J6/I6-1</f>
+        <f t="shared" si="12"/>
         <v>0.25262282416827198</v>
       </c>
       <c r="K22" s="29">
-        <f>K6/J6-1</f>
+        <f t="shared" si="12"/>
         <v>-0.19935584073076951</v>
       </c>
       <c r="L22" s="29">
-        <f>L6/K6-1</f>
+        <f t="shared" si="12"/>
         <v>0.15420436993893372</v>
       </c>
       <c r="M22" s="29">
-        <f>M6/L6-1</f>
+        <f t="shared" si="12"/>
         <v>6.692760409862708E-2</v>
       </c>
       <c r="N22" s="29">
-        <f>N6/M6-1</f>
+        <f t="shared" si="12"/>
         <v>0.18355155649811072</v>
       </c>
       <c r="O22" s="29">
-        <f>O6/N6-1</f>
+        <f t="shared" si="12"/>
         <v>-0.3003441125192895</v>
       </c>
       <c r="P22" s="29">
-        <f t="shared" ref="P22" si="12">P6/O6-1</f>
+        <f t="shared" ref="P22" si="13">P6/O6-1</f>
         <v>0.13562273171462236</v>
       </c>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
         <v>75</v>
       </c>
@@ -2978,43 +2995,43 @@
         <v>0.36754608364661018</v>
       </c>
       <c r="G24" s="29">
-        <f>G8/G6</f>
+        <f t="shared" ref="G24:O24" si="14">G8/G6</f>
         <v>5.130761366849626E-2</v>
       </c>
       <c r="H24" s="29">
-        <f>H8/H6</f>
+        <f t="shared" si="14"/>
         <v>0.30016524996887411</v>
       </c>
       <c r="I24" s="29">
-        <f>I8/I6</f>
+        <f t="shared" si="14"/>
         <v>0.4020649136258902</v>
       </c>
       <c r="J24" s="29">
-        <f>J8/J6</f>
+        <f t="shared" si="14"/>
         <v>0.34034113201473121</v>
       </c>
       <c r="K24" s="29">
-        <f>K8/K6</f>
+        <f t="shared" si="14"/>
         <v>0.42159684674670944</v>
       </c>
       <c r="L24" s="29">
-        <f>L8/L6</f>
+        <f t="shared" si="14"/>
         <v>0.42070801469824709</v>
       </c>
       <c r="M24" s="29">
-        <f>M8/M6</f>
+        <f t="shared" si="14"/>
         <v>0.44308433235641775</v>
       </c>
       <c r="N24" s="29">
-        <f>N8/N6</f>
+        <f t="shared" si="14"/>
         <v>0.32407521003861567</v>
       </c>
       <c r="O24" s="29">
-        <f>O8/O6</f>
+        <f t="shared" si="14"/>
         <v>0.36778425780328089</v>
       </c>
       <c r="P24" s="29">
-        <f t="shared" ref="P24" si="13">P8/P6</f>
+        <f t="shared" ref="P24" si="15">P8/P6</f>
         <v>0.30883030470969619</v>
       </c>
       <c r="Y24" s="29">
@@ -3026,7 +3043,7 @@
         <v>0.39750059122472825</v>
       </c>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B25" s="1" t="s">
         <v>76</v>
       </c>
@@ -3039,43 +3056,43 @@
         <v>7.8704633295512666E-2</v>
       </c>
       <c r="G25" s="29">
-        <f>G11/G6</f>
+        <f t="shared" ref="G25:O25" si="16">G11/G6</f>
         <v>-0.64934782451077766</v>
       </c>
       <c r="H25" s="29">
-        <f>H11/H6</f>
+        <f t="shared" si="16"/>
         <v>-1.3850437459677935E-2</v>
       </c>
       <c r="I25" s="29">
-        <f>I11/I6</f>
+        <f t="shared" si="16"/>
         <v>9.2622552749712247E-2</v>
       </c>
       <c r="J25" s="29">
-        <f>J11/J6</f>
+        <f t="shared" si="16"/>
         <v>2.7216580368620291E-3</v>
       </c>
       <c r="K25" s="29">
-        <f>K11/K6</f>
+        <f t="shared" si="16"/>
         <v>0.12896307221823794</v>
       </c>
       <c r="L25" s="29">
-        <f>L11/L6</f>
+        <f t="shared" si="16"/>
         <v>0.14068178696920663</v>
       </c>
       <c r="M25" s="29">
-        <f>M11/M6</f>
+        <f t="shared" si="16"/>
         <v>0.16457940565648257</v>
       </c>
       <c r="N25" s="29">
-        <f>N11/N6</f>
+        <f t="shared" si="16"/>
         <v>5.3022109013838074E-2</v>
       </c>
       <c r="O25" s="29">
-        <f>O11/O6</f>
+        <f t="shared" si="16"/>
         <v>3.9716142656608319E-2</v>
       </c>
       <c r="P25" s="29">
-        <f t="shared" ref="P25" si="14">P11/P6</f>
+        <f t="shared" ref="P25" si="17">P11/P6</f>
         <v>1.1696619047778077E-2</v>
       </c>
       <c r="Y25" s="29">
@@ -3087,7 +3104,7 @@
         <v>0.11795836380926342</v>
       </c>
     </row>
-    <row r="26" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B26" s="1" t="s">
         <v>77</v>
       </c>
@@ -3100,43 +3117,43 @@
         <v>6.2428966287147621E-2</v>
       </c>
       <c r="G26" s="29">
-        <f>G17/G6</f>
+        <f t="shared" ref="G26:O26" si="18">G17/G6</f>
         <v>-0.46613327726340054</v>
       </c>
       <c r="H26" s="29">
-        <f>H17/H6</f>
+        <f t="shared" si="18"/>
         <v>-1.5565188849022709E-2</v>
       </c>
       <c r="I26" s="29">
-        <f>I17/I6</f>
+        <f t="shared" si="18"/>
         <v>5.6327105892981497E-2</v>
       </c>
       <c r="J26" s="29">
-        <f>J17/J6</f>
+        <f t="shared" si="18"/>
         <v>2.6845128603566627E-3</v>
       </c>
       <c r="K26" s="29">
-        <f>K17/K6</f>
+        <f t="shared" si="18"/>
         <v>9.2269194114906639E-2</v>
       </c>
       <c r="L26" s="29">
-        <f>L17/L6</f>
+        <f t="shared" si="18"/>
         <v>0.10175471211466504</v>
       </c>
       <c r="M26" s="29">
-        <f>M17/M6</f>
+        <f t="shared" si="18"/>
         <v>0.11947777137663473</v>
       </c>
       <c r="N26" s="29">
-        <f>N17/N6</f>
+        <f t="shared" si="18"/>
         <v>3.3441715403229676E-2</v>
       </c>
       <c r="O26" s="29">
-        <f>O17/O6</f>
+        <f t="shared" si="18"/>
         <v>3.0084252969327211E-2</v>
       </c>
       <c r="P26" s="29">
-        <f t="shared" ref="P26" si="15">P17/P6</f>
+        <f t="shared" ref="P26" si="19">P17/P6</f>
         <v>-3.5443743719347866E-2</v>
       </c>
       <c r="Y26" s="29">
@@ -3148,7 +3165,7 @@
         <v>8.3744562977657172E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B27" s="1" t="s">
         <v>78</v>
       </c>
@@ -3161,31 +3178,31 @@
         <v>0.24363301983424923</v>
       </c>
       <c r="G27" s="29">
-        <f t="shared" ref="G27:L27" si="16">G16/G15</f>
+        <f t="shared" ref="G27:L27" si="20">G16/G15</f>
         <v>0.28836729215843088</v>
       </c>
       <c r="H27" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.28486739469578704</v>
       </c>
       <c r="I27" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.35327768503060697</v>
       </c>
       <c r="J27" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>3.185885318210679</v>
       </c>
       <c r="K27" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.24702439640009147</v>
       </c>
       <c r="L27" s="29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.24262955160248828</v>
       </c>
       <c r="M27" s="29">
-        <f t="shared" ref="M27" si="17">M16/M15</f>
+        <f t="shared" ref="M27" si="21">M16/M15</f>
         <v>0.25455302269777919</v>
       </c>
       <c r="N27" s="29">
@@ -3197,7 +3214,7 @@
         <v>0.23990612577230669</v>
       </c>
       <c r="P27" s="29">
-        <f t="shared" ref="P27" si="18">P16/P15</f>
+        <f t="shared" ref="P27" si="22">P16/P15</f>
         <v>0.10849393290506794</v>
       </c>
       <c r="Y27" s="29">
@@ -3209,12 +3226,12 @@
         <v>0.24921723759120307</v>
       </c>
     </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B29" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B30" s="38" t="s">
         <v>123</v>
       </c>
@@ -3261,7 +3278,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="31" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B31" s="38" t="s">
         <v>124</v>
       </c>
@@ -3308,7 +3325,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="32" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B32" s="38" t="s">
         <v>125</v>
       </c>
@@ -3355,7 +3372,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B33" s="38" t="s">
         <v>126</v>
       </c>
@@ -3402,7 +3419,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="34" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B34" s="38" t="s">
         <v>127</v>
       </c>
@@ -3449,7 +3466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B35" s="38" t="s">
         <v>130</v>
       </c>
@@ -3496,7 +3513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B36" s="38" t="s">
         <v>128</v>
       </c>
@@ -3543,52 +3560,52 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B37" s="38" t="s">
         <v>131</v>
       </c>
       <c r="C37" s="18">
-        <f t="shared" ref="C37:M37" si="19">C38-SUM(C30:C36)</f>
+        <f t="shared" ref="C37:M37" si="23">C38-SUM(C30:C36)</f>
         <v>6</v>
       </c>
       <c r="D37" s="18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
       <c r="E37" s="18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>7</v>
       </c>
       <c r="F37" s="18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>7</v>
       </c>
       <c r="G37" s="18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="H37" s="18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="I37" s="18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="J37" s="18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="K37" s="18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>4</v>
       </c>
       <c r="L37" s="18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
       <c r="M37" s="18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>7</v>
       </c>
       <c r="N37" s="18">
@@ -3604,7 +3621,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="2:26" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:26" s="25" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B38" s="25" t="s">
         <v>129</v>
       </c>
@@ -3663,12 +3680,12 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="40" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B40" s="32" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="2:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:26" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B41" s="2" t="s">
         <v>6</v>
       </c>
@@ -3716,7 +3733,7 @@
         <v>434.77</v>
       </c>
     </row>
-    <row r="42" spans="2:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:26" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B42" s="2" t="s">
         <v>94</v>
       </c>
@@ -3760,11 +3777,11 @@
         <v>0</v>
       </c>
       <c r="Z42" s="20">
-        <f t="shared" ref="Z42:Z43" si="20">N42</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="2:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="Z42:Z43" si="24">N42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:26" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B43" s="2" t="s">
         <v>95</v>
       </c>
@@ -3808,11 +3825,11 @@
         <v>687.04600000000005</v>
       </c>
       <c r="Z43" s="20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>553.45799999999997</v>
       </c>
     </row>
-    <row r="44" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
         <v>96</v>
       </c>
@@ -3860,7 +3877,7 @@
         <v>286.68299999999999</v>
       </c>
     </row>
-    <row r="45" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
         <v>97</v>
       </c>
@@ -3904,11 +3921,11 @@
         <v>171.32599999999999</v>
       </c>
       <c r="Z45" s="26">
-        <f t="shared" ref="Z45:Z52" si="21">N45</f>
+        <f t="shared" ref="Z45:Z52" si="25">N45</f>
         <v>122.01300000000001</v>
       </c>
     </row>
-    <row r="46" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B46" s="1" t="s">
         <v>98</v>
       </c>
@@ -3921,55 +3938,55 @@
         <v>1020.0729999999999</v>
       </c>
       <c r="F46" s="26">
-        <f t="shared" ref="F46:P46" si="22">SUM(F41:F45)</f>
+        <f t="shared" ref="F46:P46" si="26">SUM(F41:F45)</f>
         <v>1047.93</v>
       </c>
       <c r="G46" s="26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1558.9379999999999</v>
       </c>
       <c r="H46" s="26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1582.3670000000002</v>
       </c>
       <c r="I46" s="26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1507.7950000000001</v>
       </c>
       <c r="J46" s="26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1522.643</v>
       </c>
       <c r="K46" s="26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1495.78</v>
       </c>
       <c r="L46" s="26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1601.5830000000001</v>
       </c>
       <c r="M46" s="26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1775.5300000000002</v>
       </c>
       <c r="N46" s="26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1396.924</v>
       </c>
       <c r="O46" s="26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1280.539</v>
       </c>
       <c r="P46" s="26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>1177.3889999999999</v>
       </c>
       <c r="Z46" s="26">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>1396.924</v>
       </c>
     </row>
-    <row r="47" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
         <v>99</v>
       </c>
@@ -4013,11 +4030,11 @@
         <v>1210.2850000000001</v>
       </c>
       <c r="Z47" s="26">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>1193.021</v>
       </c>
     </row>
-    <row r="48" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B48" s="1" t="s">
         <v>100</v>
       </c>
@@ -4061,11 +4078,11 @@
         <v>775.96900000000005</v>
       </c>
       <c r="Z48" s="26">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>728.27200000000005</v>
       </c>
     </row>
-    <row r="49" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
         <v>101</v>
       </c>
@@ -4115,11 +4132,11 @@
         <v>370.05700000000002</v>
       </c>
       <c r="Z49" s="26">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>374.11699999999996</v>
       </c>
     </row>
-    <row r="50" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B50" s="1" t="s">
         <v>102</v>
       </c>
@@ -4163,11 +4180,11 @@
         <v>37.017000000000003</v>
       </c>
       <c r="Z50" s="26">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>44.167000000000002</v>
       </c>
     </row>
-    <row r="51" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B51" s="1" t="s">
         <v>103</v>
       </c>
@@ -4211,11 +4228,11 @@
         <v>58.5</v>
       </c>
       <c r="Z51" s="26">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>50.142000000000003</v>
       </c>
     </row>
-    <row r="52" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B52" s="1" t="s">
         <v>104</v>
       </c>
@@ -4228,55 +4245,55 @@
         <v>3359.1589999999997</v>
       </c>
       <c r="F52" s="26">
-        <f t="shared" ref="F52:P52" si="23">F46+SUM(F47:F51)</f>
+        <f t="shared" ref="F52:P52" si="27">F46+SUM(F47:F51)</f>
         <v>3328.6790000000001</v>
       </c>
       <c r="G52" s="26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>3630.1109999999999</v>
       </c>
       <c r="H52" s="26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>3627.9760000000006</v>
       </c>
       <c r="I52" s="26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>3498.2240000000002</v>
       </c>
       <c r="J52" s="26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>3434.806</v>
       </c>
       <c r="K52" s="26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>3400.6659999999997</v>
       </c>
       <c r="L52" s="26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>3495.0219999999999</v>
       </c>
       <c r="M52" s="26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>3750.0150000000003</v>
       </c>
       <c r="N52" s="26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>3786.6429999999996</v>
       </c>
       <c r="O52" s="26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>3701.518</v>
       </c>
       <c r="P52" s="26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>3629.2169999999996</v>
       </c>
       <c r="Z52" s="26">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>3786.6429999999996</v>
       </c>
     </row>
-    <row r="53" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:26" x14ac:dyDescent="0.15">
       <c r="D53" s="26"/>
       <c r="F53" s="26"/>
       <c r="G53" s="26"/>
@@ -4284,7 +4301,7 @@
       <c r="M53" s="26"/>
       <c r="N53" s="26"/>
     </row>
-    <row r="54" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B54" s="1" t="s">
         <v>105</v>
       </c>
@@ -4332,7 +4349,7 @@
         <v>231.78200000000001</v>
       </c>
     </row>
-    <row r="55" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B55" s="1" t="s">
         <v>106</v>
       </c>
@@ -4376,11 +4393,11 @@
         <v>328.34800000000001</v>
       </c>
       <c r="Z55" s="26">
-        <f t="shared" ref="Z55:Z70" si="24">N55</f>
+        <f t="shared" ref="Z55:Z70" si="28">N55</f>
         <v>311.005</v>
       </c>
     </row>
-    <row r="56" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B56" s="1" t="s">
         <v>107</v>
       </c>
@@ -4424,11 +4441,11 @@
         <v>51.110999999999997</v>
       </c>
       <c r="Z56" s="26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>71.364999999999995</v>
       </c>
     </row>
-    <row r="57" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B57" s="1" t="s">
         <v>108</v>
       </c>
@@ -4472,11 +4489,11 @@
         <v>50.787999999999997</v>
       </c>
       <c r="Z57" s="26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>141.81700000000001</v>
       </c>
     </row>
-    <row r="58" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B58" s="1" t="s">
         <v>109</v>
       </c>
@@ -4521,11 +4538,11 @@
         <v>16.707999999999998</v>
       </c>
       <c r="Z58" s="26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>16.274000000000001</v>
       </c>
     </row>
-    <row r="59" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B59" s="1" t="s">
         <v>110</v>
       </c>
@@ -4570,11 +4587,11 @@
         <v>72.460999999999999</v>
       </c>
       <c r="Z59" s="26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>70.628</v>
       </c>
     </row>
-    <row r="60" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B60" s="1" t="s">
         <v>111</v>
       </c>
@@ -4587,55 +4604,55 @@
         <v>1025.0989999999999</v>
       </c>
       <c r="F60" s="26">
-        <f t="shared" ref="F60:P60" si="25">SUM(F54:F59)</f>
+        <f t="shared" ref="F60:P60" si="29">SUM(F54:F59)</f>
         <v>751.75599999999997</v>
       </c>
       <c r="G60" s="26">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>662.22699999999998</v>
       </c>
       <c r="H60" s="26">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>840.41399999999987</v>
       </c>
       <c r="I60" s="26">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>871.49300000000005</v>
       </c>
       <c r="J60" s="26">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>858.48199999999997</v>
       </c>
       <c r="K60" s="26">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>744.73299999999995</v>
       </c>
       <c r="L60" s="26">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>769.21800000000007</v>
       </c>
       <c r="M60" s="26">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>869.572</v>
       </c>
       <c r="N60" s="26">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>842.87100000000009</v>
       </c>
       <c r="O60" s="26">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>737.47900000000004</v>
       </c>
       <c r="P60" s="26">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>718.06100000000004</v>
       </c>
       <c r="Z60" s="26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>842.87100000000009</v>
       </c>
     </row>
-    <row r="61" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B61" s="1" t="s">
         <v>119</v>
       </c>
@@ -4679,11 +4696,11 @@
         <v>1137.6559999999999</v>
       </c>
       <c r="Z61" s="26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>1154.481</v>
       </c>
     </row>
-    <row r="62" spans="2:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:26" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B62" s="2" t="s">
         <v>112</v>
       </c>
@@ -4731,7 +4748,7 @@
         <v>341.00200000000001</v>
       </c>
     </row>
-    <row r="63" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B63" s="1" t="s">
         <v>113</v>
       </c>
@@ -4775,11 +4792,11 @@
         <v>24.055</v>
       </c>
       <c r="Z63" s="26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>24.617000000000001</v>
       </c>
     </row>
-    <row r="64" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B64" s="1" t="s">
         <v>114</v>
       </c>
@@ -4792,55 +4809,55 @@
         <v>2392.0350000000003</v>
       </c>
       <c r="F64" s="26">
-        <f t="shared" ref="F64:P64" si="26">F60+F61+F62+F63</f>
+        <f t="shared" ref="F64:P64" si="30">F60+F61+F62+F63</f>
         <v>2080.826</v>
       </c>
       <c r="G64" s="26">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>2633.1279999999997</v>
       </c>
       <c r="H64" s="26">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>2630.0729999999999</v>
       </c>
       <c r="I64" s="26">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>2407.1750000000002</v>
       </c>
       <c r="J64" s="26">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>2348.1410000000001</v>
       </c>
       <c r="K64" s="26">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>2225.3530000000001</v>
       </c>
       <c r="L64" s="26">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>2219.491</v>
       </c>
       <c r="M64" s="26">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>2353.3180000000002</v>
       </c>
       <c r="N64" s="26">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>2362.9710000000005</v>
       </c>
       <c r="O64" s="26">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>2318.5120000000002</v>
       </c>
       <c r="P64" s="26">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>2256.2939999999999</v>
       </c>
       <c r="Z64" s="26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>2362.9710000000005</v>
       </c>
     </row>
-    <row r="65" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:26" x14ac:dyDescent="0.15">
       <c r="C65" s="26"/>
       <c r="D65" s="26"/>
       <c r="I65" s="26"/>
@@ -4848,7 +4865,7 @@
       <c r="M65" s="26"/>
       <c r="N65" s="26"/>
     </row>
-    <row r="66" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B66" s="1" t="s">
         <v>115</v>
       </c>
@@ -4892,11 +4909,11 @@
         <v>1372.923</v>
       </c>
       <c r="Z66" s="26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>1423.672</v>
       </c>
     </row>
-    <row r="67" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B67" s="1" t="s">
         <v>116</v>
       </c>
@@ -4909,104 +4926,104 @@
         <v>3620.6120000000001</v>
       </c>
       <c r="F67" s="26">
-        <f t="shared" ref="F67:P67" si="27">F66+F64</f>
+        <f t="shared" ref="F67:P67" si="31">F66+F64</f>
         <v>3328.6790000000001</v>
       </c>
       <c r="G67" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3630.1109999999999</v>
       </c>
       <c r="H67" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3627.973</v>
       </c>
       <c r="I67" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3475.3720000000003</v>
       </c>
       <c r="J67" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3434.806</v>
       </c>
       <c r="K67" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3400.9160000000002</v>
       </c>
       <c r="L67" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3495.0219999999999</v>
       </c>
       <c r="M67" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3750.0150000000003</v>
       </c>
       <c r="N67" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3786.6430000000005</v>
       </c>
       <c r="O67" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3701.518</v>
       </c>
       <c r="P67" s="26">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>3629.2169999999996</v>
       </c>
       <c r="Z67" s="26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>3786.6430000000005</v>
       </c>
     </row>
-    <row r="68" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:26" x14ac:dyDescent="0.15">
       <c r="I68" s="26"/>
       <c r="L68" s="26"/>
     </row>
-    <row r="69" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B69" s="1" t="s">
         <v>117</v>
       </c>
       <c r="C69" s="26">
-        <f t="shared" ref="C69" si="28">C52-C64</f>
+        <f t="shared" ref="C69" si="32">C52-C64</f>
         <v>1241.751</v>
       </c>
       <c r="D69" s="26">
-        <f t="shared" ref="D69:G69" si="29">D52-D64</f>
+        <f t="shared" ref="D69:G69" si="33">D52-D64</f>
         <v>967.12399999999934</v>
       </c>
       <c r="F69" s="26">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>1247.8530000000001</v>
       </c>
       <c r="G69" s="26">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>996.98300000000017</v>
       </c>
       <c r="H69" s="26">
-        <f t="shared" ref="H69:I69" si="30">H52-H64</f>
+        <f t="shared" ref="H69:I69" si="34">H52-H64</f>
         <v>997.9030000000007</v>
       </c>
       <c r="I69" s="26">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>1091.049</v>
       </c>
       <c r="J69" s="26">
-        <f t="shared" ref="J69:K69" si="31">J52-J64</f>
+        <f t="shared" ref="J69:K69" si="35">J52-J64</f>
         <v>1086.665</v>
       </c>
       <c r="K69" s="26">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>1175.3129999999996</v>
       </c>
       <c r="L69" s="26">
-        <f t="shared" ref="L69:M69" si="32">L52-L64</f>
+        <f t="shared" ref="L69:M69" si="36">L52-L64</f>
         <v>1275.5309999999999</v>
       </c>
       <c r="M69" s="26">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>1396.6970000000001</v>
       </c>
       <c r="N69" s="26">
-        <f t="shared" ref="N69" si="33">N52-N64</f>
+        <f t="shared" ref="N69" si="37">N52-N64</f>
         <v>1423.6719999999991</v>
       </c>
       <c r="O69" s="26">
@@ -5014,15 +5031,15 @@
         <v>1383.0059999999999</v>
       </c>
       <c r="P69" s="26">
-        <f t="shared" ref="P69" si="34">P52-P64</f>
+        <f t="shared" ref="P69" si="38">P52-P64</f>
         <v>1372.9229999999998</v>
       </c>
       <c r="Z69" s="26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>1423.6719999999991</v>
       </c>
     </row>
-    <row r="70" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B70" s="1" t="s">
         <v>118</v>
       </c>
@@ -5036,69 +5053,69 @@
       </c>
       <c r="F70" s="26"/>
       <c r="G70" s="26">
-        <f t="shared" ref="F70:O70" si="35">G69/G19</f>
+        <f t="shared" ref="G70:O70" si="39">G69/G19</f>
         <v>5.9777972310994665</v>
       </c>
       <c r="H70" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>6.0000781649280022</v>
       </c>
       <c r="I70" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>6.5652676234317173</v>
       </c>
       <c r="J70" s="27">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>6.5339727015813835</v>
       </c>
       <c r="K70" s="27">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>7.0269884070621833</v>
       </c>
       <c r="L70" s="27">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>7.6155196398612457</v>
       </c>
       <c r="M70" s="27">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>8.3316749882185928</v>
       </c>
       <c r="N70" s="27">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>8.4939055312598768</v>
       </c>
       <c r="O70" s="27">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>8.2096996319601079</v>
       </c>
       <c r="P70" s="27">
-        <f t="shared" ref="P70" si="36">P69/P19</f>
+        <f t="shared" ref="P70" si="40">P69/P19</f>
         <v>7.6193496828330245</v>
       </c>
       <c r="Z70" s="26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>8.4939055312598768</v>
       </c>
     </row>
-    <row r="72" spans="2:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:26" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B72" s="2" t="s">
         <v>120</v>
       </c>
       <c r="G72" s="28">
-        <f t="shared" ref="G72:K72" si="37">G43/C43-1</f>
+        <f t="shared" ref="G72:K72" si="41">G43/C43-1</f>
         <v>-7.5480094703612832E-2</v>
       </c>
       <c r="H72" s="28">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-0.21236737090518765</v>
       </c>
       <c r="I72" s="28"/>
       <c r="J72" s="28">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-9.1496780033969882E-2</v>
       </c>
       <c r="K72" s="28">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>0.10663008709384458</v>
       </c>
       <c r="L72" s="28">
@@ -5118,54 +5135,54 @@
         <v>0.4615447248541884</v>
       </c>
       <c r="P72" s="28">
-        <f t="shared" ref="P72" si="38">P43/L43-1</f>
+        <f t="shared" ref="P72" si="42">P43/L43-1</f>
         <v>0.36452124796676122</v>
       </c>
       <c r="Z72" s="26"/>
     </row>
-    <row r="73" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B73" s="1" t="s">
         <v>121</v>
       </c>
       <c r="D73" s="29">
-        <f t="shared" ref="D73:E73" si="39">D43/C43-1</f>
+        <f t="shared" ref="D73:E73" si="43">D43/C43-1</f>
         <v>0.17231234654507177</v>
       </c>
       <c r="E73" s="29">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-1</v>
       </c>
       <c r="F73" s="29"/>
       <c r="G73" s="29">
-        <f t="shared" ref="F73:K73" si="40">G43/F43-1</f>
+        <f t="shared" ref="G73:K73" si="44">G43/F43-1</f>
         <v>-5.5008313203877446E-2</v>
       </c>
       <c r="H73" s="29">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-1.2638447913232431E-3</v>
       </c>
       <c r="I73" s="29">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>0.32945469567612218</v>
       </c>
       <c r="J73" s="29">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-0.27594064586640854</v>
       </c>
       <c r="K73" s="29">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>0.15107597824612462</v>
       </c>
       <c r="L73" s="29">
-        <f t="shared" ref="L73:N73" si="41">L43/K43-1</f>
+        <f t="shared" ref="L73:N73" si="45">L43/K43-1</f>
         <v>7.8871132938217015E-2</v>
       </c>
       <c r="M73" s="29">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0.4693102578514301</v>
       </c>
       <c r="N73" s="29">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-0.25188967948440677</v>
       </c>
       <c r="O73" s="29">
@@ -5173,7 +5190,7 @@
         <v>0.23243317469437619</v>
       </c>
       <c r="P73" s="29">
-        <f t="shared" ref="P73" si="42">P43/O43-1</f>
+        <f t="shared" ref="P73" si="46">P43/O43-1</f>
         <v>7.2511361970386545E-3</v>
       </c>
       <c r="X73" s="42" t="s">
@@ -5186,60 +5203,60 @@
         <v>134</v>
       </c>
     </row>
-    <row r="75" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B75" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C75" s="19">
-        <f t="shared" ref="C75:O75" si="43">C41+C42</f>
+        <f t="shared" ref="C75:O75" si="47">C41+C42</f>
         <v>349.67099999999999</v>
       </c>
       <c r="D75" s="19">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>317.166</v>
       </c>
       <c r="E75" s="19">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="F75" s="19">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>416.93</v>
       </c>
       <c r="G75" s="19">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>885.72500000000002</v>
       </c>
       <c r="H75" s="19">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>898.78700000000003</v>
       </c>
       <c r="I75" s="19">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>692.36500000000001</v>
       </c>
       <c r="J75" s="19">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>850.47699999999998</v>
       </c>
       <c r="K75" s="19">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>791.67899999999997</v>
       </c>
       <c r="L75" s="19">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>823.99400000000003</v>
       </c>
       <c r="M75" s="19">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>740.66800000000001</v>
       </c>
       <c r="N75" s="19">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>434.77</v>
       </c>
       <c r="O75" s="19">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>228.77500000000001</v>
       </c>
       <c r="P75" s="19">
@@ -5247,60 +5264,60 @@
         <v>98.213999999999999</v>
       </c>
       <c r="Z75" s="19">
-        <f t="shared" ref="Z75" si="44">Z41+Z42</f>
+        <f t="shared" ref="Z75" si="48">Z41+Z42</f>
         <v>434.77</v>
       </c>
     </row>
-    <row r="76" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:26" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B76" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C76" s="19">
-        <f t="shared" ref="C76:D76" si="45">+C62</f>
+        <f t="shared" ref="C76:D76" si="49">+C62</f>
         <v>0</v>
       </c>
       <c r="D76" s="19">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="F76" s="19">
-        <f t="shared" ref="F76:P76" si="46">+F62</f>
+        <f t="shared" ref="F76:O76" si="50">+F62</f>
         <v>0</v>
       </c>
       <c r="G76" s="19">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>642.97199999999998</v>
       </c>
       <c r="H76" s="19">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>516.95299999999997</v>
       </c>
       <c r="I76" s="19">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>321.08100000000002</v>
       </c>
       <c r="J76" s="19">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>325.29000000000002</v>
       </c>
       <c r="K76" s="19">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>329.71800000000002</v>
       </c>
       <c r="L76" s="19">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>331.68</v>
       </c>
       <c r="M76" s="19">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>336.24900000000002</v>
       </c>
       <c r="N76" s="19">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>341.00200000000001</v>
       </c>
       <c r="O76" s="19">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>405.80700000000002</v>
       </c>
       <c r="P76" s="19">
@@ -5308,60 +5325,60 @@
         <v>376.52199999999999</v>
       </c>
       <c r="Z76" s="19">
-        <f t="shared" ref="Z76" si="47">+Z62</f>
+        <f t="shared" ref="Z76" si="51">+Z62</f>
         <v>341.00200000000001</v>
       </c>
     </row>
-    <row r="77" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B77" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C77" s="26">
-        <f t="shared" ref="C77" si="48">C75-C76</f>
+        <f t="shared" ref="C77" si="52">C75-C76</f>
         <v>349.67099999999999</v>
       </c>
       <c r="D77" s="26">
-        <f t="shared" ref="D77:O77" si="49">D75-D76</f>
+        <f t="shared" ref="D77:O77" si="53">D75-D76</f>
         <v>317.166</v>
       </c>
       <c r="F77" s="26">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>416.93</v>
       </c>
       <c r="G77" s="26">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>242.75300000000004</v>
       </c>
       <c r="H77" s="26">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>381.83400000000006</v>
       </c>
       <c r="I77" s="26">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>371.28399999999999</v>
       </c>
       <c r="J77" s="26">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>525.1869999999999</v>
       </c>
       <c r="K77" s="26">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>461.96099999999996</v>
       </c>
       <c r="L77" s="26">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>492.31400000000002</v>
       </c>
       <c r="M77" s="26">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>404.41899999999998</v>
       </c>
       <c r="N77" s="26">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>93.767999999999972</v>
       </c>
       <c r="O77" s="26">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>-177.03200000000001</v>
       </c>
       <c r="P77" s="26">
@@ -5369,11 +5386,11 @@
         <v>-278.30799999999999</v>
       </c>
       <c r="Z77" s="26">
-        <f t="shared" ref="Z77" si="50">Z75-Z76</f>
+        <f t="shared" ref="Z77" si="54">Z75-Z76</f>
         <v>93.767999999999972</v>
       </c>
     </row>
-    <row r="79" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B79" s="1" t="s">
         <v>136</v>
       </c>
@@ -5421,56 +5438,56 @@
         <v>22.25</v>
       </c>
     </row>
-    <row r="80" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:26" x14ac:dyDescent="0.15">
       <c r="B80" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C80" s="26">
-        <f t="shared" ref="C80" si="51">C79*C19</f>
+        <f t="shared" ref="C80" si="55">C79*C19</f>
         <v>3860.93914</v>
       </c>
       <c r="D80" s="26">
-        <f t="shared" ref="D80" si="52">D79*D19</f>
+        <f t="shared" ref="D80" si="56">D79*D19</f>
         <v>2605.91777</v>
       </c>
       <c r="F80" s="26">
-        <f t="shared" ref="F80:O80" si="53">F79*F19</f>
+        <f t="shared" ref="F80:O80" si="57">F79*F19</f>
         <v>0</v>
       </c>
       <c r="G80" s="26">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>1444.3234600000001</v>
       </c>
       <c r="H80" s="26">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>1982.4748</v>
       </c>
       <c r="I80" s="26">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>2153.7576000000004</v>
       </c>
       <c r="J80" s="26">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>3592.2960000000003</v>
       </c>
       <c r="K80" s="26">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>5666.6671600000009</v>
       </c>
       <c r="L80" s="26">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>5548.9768300000005</v>
       </c>
       <c r="M80" s="26">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>3853.9746299999997</v>
       </c>
       <c r="N80" s="26">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>3729.3447499999997</v>
       </c>
       <c r="O80" s="26">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>2506.6848000000005</v>
       </c>
       <c r="P80" s="26">
@@ -5478,60 +5495,60 @@
         <v>2169.4755599999999</v>
       </c>
       <c r="Z80" s="26">
-        <f t="shared" ref="Z80" si="54">Z79*Z19</f>
+        <f t="shared" ref="Z80" si="58">Z79*Z19</f>
         <v>3729.3447499999997</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B81" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C81" s="26">
-        <f t="shared" ref="C81" si="55">C80-C77</f>
+        <f t="shared" ref="C81" si="59">C80-C77</f>
         <v>3511.2681400000001</v>
       </c>
       <c r="D81" s="26">
-        <f t="shared" ref="D81" si="56">D80-D77</f>
+        <f t="shared" ref="D81" si="60">D80-D77</f>
         <v>2288.7517699999999</v>
       </c>
       <c r="F81" s="26">
-        <f t="shared" ref="F81:O81" si="57">F80-F77</f>
+        <f t="shared" ref="F81:O81" si="61">F80-F77</f>
         <v>-416.93</v>
       </c>
       <c r="G81" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>1201.5704599999999</v>
       </c>
       <c r="H81" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>1600.6407999999999</v>
       </c>
       <c r="I81" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>1782.4736000000003</v>
       </c>
       <c r="J81" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>3067.1090000000004</v>
       </c>
       <c r="K81" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>5204.7061600000006</v>
       </c>
       <c r="L81" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>5056.6628300000002</v>
       </c>
       <c r="M81" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>3449.5556299999998</v>
       </c>
       <c r="N81" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>3635.5767499999997</v>
       </c>
       <c r="O81" s="26">
-        <f t="shared" si="57"/>
+        <f t="shared" si="61"/>
         <v>2683.7168000000006</v>
       </c>
       <c r="P81" s="26">
@@ -5539,264 +5556,305 @@
         <v>2447.7835599999999</v>
       </c>
       <c r="Z81" s="26">
-        <f t="shared" ref="Z81" si="58">Z80-Z77</f>
+        <f t="shared" ref="Z81" si="62">Z80-Z77</f>
         <v>3635.5767499999997</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A83" s="59">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A83" s="46">
         <f>AVERAGE(C83:P83)</f>
         <v>2.7051850562149427</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C83" s="58">
-        <f t="shared" ref="C83:P83" si="59">C79/C70</f>
+      <c r="C83" s="45">
+        <f t="shared" ref="C83:O83" si="63">C79/C70</f>
         <v>3.1092700066277379</v>
       </c>
-      <c r="D83" s="58">
-        <f t="shared" si="59"/>
+      <c r="D83" s="45">
+        <f t="shared" si="63"/>
         <v>2.6945022251541704</v>
       </c>
-      <c r="E83" s="58"/>
-      <c r="F83" s="58"/>
-      <c r="G83" s="58">
-        <f t="shared" si="59"/>
+      <c r="E83" s="45"/>
+      <c r="F83" s="45"/>
+      <c r="G83" s="45">
+        <f t="shared" si="63"/>
         <v>1.4486941703118306</v>
       </c>
-      <c r="H83" s="58">
-        <f t="shared" si="59"/>
+      <c r="H83" s="45">
+        <f t="shared" si="63"/>
         <v>1.9866407857276696</v>
       </c>
-      <c r="I83" s="58">
-        <f t="shared" si="59"/>
+      <c r="I83" s="45">
+        <f t="shared" si="63"/>
         <v>1.9740246313410308</v>
       </c>
-      <c r="J83" s="58">
-        <f t="shared" si="59"/>
+      <c r="J83" s="45">
+        <f t="shared" si="63"/>
         <v>3.3057989352744412</v>
       </c>
-      <c r="K83" s="58">
-        <f t="shared" si="59"/>
+      <c r="K83" s="45">
+        <f t="shared" si="63"/>
         <v>4.8214111134650963</v>
       </c>
-      <c r="L83" s="58">
-        <f t="shared" si="59"/>
+      <c r="L83" s="45">
+        <f t="shared" si="63"/>
         <v>4.3503269069901087</v>
       </c>
-      <c r="M83" s="58">
-        <f t="shared" si="59"/>
+      <c r="M83" s="45">
+        <f t="shared" si="63"/>
         <v>2.7593491143748423</v>
       </c>
-      <c r="N83" s="58">
-        <f t="shared" si="59"/>
+      <c r="N83" s="45">
+        <f t="shared" si="63"/>
         <v>2.6195252487932628</v>
       </c>
-      <c r="O83" s="58">
-        <f t="shared" si="59"/>
+      <c r="O83" s="45">
+        <f t="shared" si="63"/>
         <v>1.812490184424363</v>
       </c>
-      <c r="P83" s="58">
+      <c r="P83" s="45">
         <f>P79/P70</f>
         <v>1.5801873520947642</v>
       </c>
-      <c r="Z83" s="58">
+      <c r="Z83" s="45">
         <f>Z79/Z70</f>
         <v>2.6195252487932628</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A84" s="59">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A84" s="46">
         <f>AVERAGE(C84:P84)</f>
         <v>0.8553491796573508</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="J84" s="58">
-        <f t="shared" ref="J84:O84" si="60">J80/SUM(G6:J6)</f>
+      <c r="J84" s="45">
+        <f t="shared" ref="J84:O84" si="64">J80/SUM(G6:J6)</f>
         <v>0.95564034066090175</v>
       </c>
-      <c r="K84" s="58">
-        <f t="shared" si="60"/>
+      <c r="K84" s="45">
+        <f t="shared" si="64"/>
         <v>1.3358580639929392</v>
       </c>
-      <c r="L84" s="58">
-        <f t="shared" si="60"/>
+      <c r="L84" s="45">
+        <f t="shared" si="64"/>
         <v>1.2188551082960253</v>
       </c>
-      <c r="M84" s="58">
-        <f t="shared" si="60"/>
+      <c r="M84" s="45">
+        <f t="shared" si="64"/>
         <v>0.80373604792417197</v>
       </c>
-      <c r="N84" s="58">
-        <f t="shared" si="60"/>
+      <c r="N84" s="45">
+        <f t="shared" si="64"/>
         <v>0.74426357347202077</v>
       </c>
-      <c r="O84" s="58">
-        <f t="shared" si="60"/>
+      <c r="O84" s="45">
+        <f t="shared" si="64"/>
         <v>0.49822722495273514</v>
       </c>
-      <c r="P84" s="58">
+      <c r="P84" s="45">
         <f>P80/SUM(M6:P6)</f>
         <v>0.43086389830266114</v>
       </c>
-      <c r="Z84" s="58">
+      <c r="Z84" s="45">
         <f>Z80/Z6</f>
         <v>0.74426357347202077</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A85" s="59">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A85" s="46">
         <f>AVERAGE(C85:P85)</f>
         <v>0.80258513379488117</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J85" s="58">
-        <f t="shared" ref="J85:O85" si="61">J81/SUM(G6:J6)</f>
+      <c r="J85" s="45">
+        <f t="shared" ref="J85:O85" si="65">J81/SUM(G6:J6)</f>
         <v>0.81592749862598124</v>
       </c>
-      <c r="K85" s="58">
-        <f t="shared" si="61"/>
+      <c r="K85" s="45">
+        <f t="shared" si="65"/>
         <v>1.2269555451620568</v>
       </c>
-      <c r="L85" s="58">
-        <f t="shared" si="61"/>
+      <c r="L85" s="45">
+        <f t="shared" si="65"/>
         <v>1.1107163554828063</v>
       </c>
-      <c r="M85" s="58">
-        <f t="shared" si="61"/>
+      <c r="M85" s="45">
+        <f t="shared" si="65"/>
         <v>0.71939555272858069</v>
       </c>
-      <c r="N85" s="58">
-        <f t="shared" si="61"/>
+      <c r="N85" s="45">
+        <f t="shared" si="65"/>
         <v>0.72555033792110413</v>
       </c>
-      <c r="O85" s="58">
-        <f t="shared" si="61"/>
+      <c r="O85" s="45">
+        <f t="shared" si="65"/>
         <v>0.53341400315788989</v>
       </c>
-      <c r="P85" s="58">
+      <c r="P85" s="45">
         <f>P81/SUM(M6:P6)</f>
         <v>0.48613664348574909</v>
       </c>
-      <c r="Z85" s="58">
+      <c r="Z85" s="45">
         <f>Z81/Z6</f>
         <v>0.72555033792110413</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A86" s="59">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A86" s="46">
         <f>AVERAGE(C86:P86)</f>
         <v>38.697690419113108</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J86" s="58"/>
-      <c r="K86" s="58">
-        <f t="shared" ref="J86:O86" si="62">K79/(H18:K18)</f>
+      <c r="J86" s="45"/>
+      <c r="K86" s="45">
+        <f t="shared" ref="K86:O86" si="66">K79/(H18:K18)</f>
         <v>59.359826948660725</v>
       </c>
-      <c r="L86" s="58">
-        <f t="shared" si="62"/>
+      <c r="L86" s="45">
+        <f t="shared" si="66"/>
         <v>45.66645678169057</v>
       </c>
-      <c r="M86" s="58">
-        <f t="shared" si="62"/>
+      <c r="M86" s="45">
+        <f t="shared" si="66"/>
         <v>25.317785828778636</v>
       </c>
-      <c r="N86" s="58">
-        <f t="shared" si="62"/>
+      <c r="N86" s="45">
+        <f t="shared" si="66"/>
         <v>73.953850043626645</v>
       </c>
-      <c r="O86" s="58">
-        <f t="shared" si="62"/>
+      <c r="O86" s="45">
+        <f t="shared" si="66"/>
         <v>78.975576559546141</v>
       </c>
-      <c r="P86" s="58">
+      <c r="P86" s="45">
         <f>P79/(M18:P18)</f>
         <v>-51.087353647624042</v>
       </c>
-      <c r="Z86" s="58">
+      <c r="Z86" s="45">
         <f>Z79/Z18</f>
         <v>8.8873061964701936</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A87" s="59">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A87" s="46">
         <f>AVERAGE(C87:P87)</f>
         <v>15.448578569458997</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K87" s="58">
-        <f t="shared" ref="K87:O87" si="63">K81/SUM(H17:K17)</f>
+      <c r="K87" s="45">
+        <f t="shared" ref="K87:O87" si="67">K81/SUM(H17:K17)</f>
         <v>36.323391770420429</v>
       </c>
-      <c r="L87" s="58">
-        <f t="shared" si="63"/>
+      <c r="L87" s="45">
+        <f t="shared" si="67"/>
         <v>18.153454232797589</v>
       </c>
-      <c r="M87" s="58">
-        <f t="shared" si="63"/>
+      <c r="M87" s="45">
+        <f t="shared" si="67"/>
         <v>9.2564021767422364</v>
       </c>
-      <c r="N87" s="58">
-        <f t="shared" si="63"/>
+      <c r="N87" s="45">
+        <f t="shared" si="67"/>
         <v>8.6638500712539273</v>
       </c>
-      <c r="O87" s="58">
-        <f t="shared" si="63"/>
+      <c r="O87" s="45">
+        <f t="shared" si="67"/>
         <v>7.5405849346591651</v>
       </c>
-      <c r="P87" s="58">
+      <c r="P87" s="45">
         <f>P81/SUM(M17:P17)</f>
         <v>12.753788230880646</v>
       </c>
-      <c r="Z87" s="58">
+      <c r="Z87" s="45">
         <f>Z81/Z17</f>
         <v>8.663850071253929</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B89" s="1" t="s">
+    <row r="88" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A88" s="62">
+        <f>AVERAGE(C88:P88)</f>
+        <v>0.23544875859612088</v>
+      </c>
+      <c r="B88" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="J88" s="29">
+        <f t="shared" ref="H88:O88" si="68">SUM(G11:J11)/J69</f>
+        <v>-0.24976326650807743</v>
+      </c>
+      <c r="K88" s="29">
+        <f t="shared" si="68"/>
+        <v>0.18740369586654793</v>
+      </c>
+      <c r="L88" s="29">
+        <f t="shared" si="68"/>
+        <v>0.3139798248729353</v>
+      </c>
+      <c r="M88" s="29">
+        <f t="shared" si="68"/>
+        <v>0.36846001673949325</v>
+      </c>
+      <c r="N88" s="29">
+        <f t="shared" si="68"/>
+        <v>0.41516866244472056</v>
+      </c>
+      <c r="O88" s="29">
+        <f t="shared" si="68"/>
+        <v>0.36119799914100159</v>
+      </c>
+      <c r="P88" s="29">
+        <f>SUM(M11:P11)/P69</f>
+        <v>0.25169437761622476</v>
+      </c>
+      <c r="Z88" s="29">
+        <f>Z11/Z69</f>
+        <v>0.41516866244472067</v>
+      </c>
+    </row>
+    <row r="90" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="B90" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C89" s="29"/>
-      <c r="D89" s="29">
-        <f t="shared" ref="D89" si="64">D43/SUM(A6:D6)</f>
+      <c r="C90" s="29"/>
+      <c r="D90" s="29">
+        <f t="shared" ref="D90" si="69">D43/SUM(A6:D6)</f>
         <v>0.2774857835508977</v>
       </c>
-      <c r="J89" s="29">
-        <f t="shared" ref="J89:O89" si="65">J43/SUM(G6:J6)</f>
+      <c r="J90" s="29">
+        <f t="shared" ref="J90:O90" si="70">J43/SUM(G6:J6)</f>
         <v>0.10785848324282277</v>
       </c>
-      <c r="K89" s="29">
-        <f t="shared" si="65"/>
+      <c r="K90" s="29">
+        <f t="shared" si="70"/>
         <v>0.11001921749527575</v>
       </c>
-      <c r="L89" s="29">
-        <f t="shared" si="65"/>
+      <c r="L90" s="29">
+        <f t="shared" si="70"/>
         <v>0.11059734034117544</v>
       </c>
-      <c r="M89" s="29">
-        <f t="shared" si="65"/>
+      <c r="M90" s="29">
+        <f t="shared" si="70"/>
         <v>0.15428496947388726</v>
       </c>
-      <c r="N89" s="29">
-        <f t="shared" si="65"/>
+      <c r="N90" s="29">
+        <f t="shared" si="70"/>
         <v>0.11045335211947828</v>
       </c>
-      <c r="O89" s="29">
-        <f t="shared" si="65"/>
+      <c r="O90" s="29">
+        <f t="shared" si="70"/>
         <v>0.13557380255397911</v>
       </c>
-      <c r="P89" s="29">
+      <c r="P90" s="29">
         <f>P43/SUM(M6:P6)</f>
         <v>0.13644925222077642</v>
       </c>

</xml_diff>